<commit_message>
copying the donor ids into source for NDDs in data sample, testing RA on data
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burlt\Downloads\Topics of Applied Operational Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1975950\Desktop\taor_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{796412D2-E1F4-4294-A74F-8C4CEAC77438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBB5DD2-E7AF-4D42-82C1-EBBB291DA7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0DAAF120-E45A-4444-8930-A3E6281725AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0DAAF120-E45A-4444-8930-A3E6281725AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,19 +494,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="C246" sqref="C246:C263"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -537,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -554,7 +556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1</v>
       </c>
@@ -571,7 +573,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
@@ -588,7 +590,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1</v>
       </c>
@@ -605,7 +607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>1</v>
       </c>
@@ -622,7 +624,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1</v>
       </c>
@@ -639,7 +641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1</v>
       </c>
@@ -656,7 +658,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1</v>
       </c>
@@ -673,7 +675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1</v>
       </c>
@@ -690,7 +692,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>1</v>
       </c>
@@ -707,7 +709,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>1</v>
       </c>
@@ -724,7 +726,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>2</v>
       </c>
@@ -741,7 +743,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2</v>
       </c>
@@ -758,7 +760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>2</v>
       </c>
@@ -775,7 +777,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -792,7 +794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
@@ -809,7 +811,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2</v>
       </c>
@@ -826,7 +828,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2</v>
       </c>
@@ -843,7 +845,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2</v>
       </c>
@@ -860,7 +862,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2</v>
       </c>
@@ -877,7 +879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2</v>
       </c>
@@ -894,7 +896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>3</v>
       </c>
@@ -911,7 +913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>3</v>
       </c>
@@ -928,7 +930,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>4</v>
       </c>
@@ -945,7 +947,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>5</v>
       </c>
@@ -962,7 +964,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>5</v>
       </c>
@@ -979,7 +981,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>5</v>
       </c>
@@ -996,7 +998,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1013,7 +1015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>5</v>
       </c>
@@ -1030,7 +1032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1047,7 +1049,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>5</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>5</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>5</v>
       </c>
@@ -1098,7 +1100,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1115,7 +1117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1132,7 +1134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1149,7 +1151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>7</v>
       </c>
@@ -1166,7 +1168,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>7</v>
       </c>
@@ -1183,7 +1185,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>8</v>
       </c>
@@ -1200,7 +1202,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>8</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>8</v>
       </c>
@@ -1234,7 +1236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>8</v>
       </c>
@@ -1251,7 +1253,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>8</v>
       </c>
@@ -1268,7 +1270,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>9</v>
       </c>
@@ -1285,7 +1287,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>9</v>
       </c>
@@ -1302,7 +1304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>10</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>10</v>
       </c>
@@ -1336,7 +1338,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>11</v>
       </c>
@@ -1353,7 +1355,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>11</v>
       </c>
@@ -1370,7 +1372,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>12</v>
       </c>
@@ -1387,7 +1389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>12</v>
       </c>
@@ -1404,7 +1406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>12</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>13</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>13</v>
       </c>
@@ -1455,7 +1457,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>13</v>
       </c>
@@ -1472,7 +1474,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>13</v>
       </c>
@@ -1489,7 +1491,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>13</v>
       </c>
@@ -1506,7 +1508,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>13</v>
       </c>
@@ -1523,7 +1525,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>13</v>
       </c>
@@ -1540,7 +1542,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>13</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>13</v>
       </c>
@@ -1574,7 +1576,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>13</v>
       </c>
@@ -1591,7 +1593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>14</v>
       </c>
@@ -1608,7 +1610,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>14</v>
       </c>
@@ -1625,7 +1627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>14</v>
       </c>
@@ -1642,7 +1644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>14</v>
       </c>
@@ -1659,7 +1661,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>14</v>
       </c>
@@ -1676,7 +1678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>14</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>14</v>
       </c>
@@ -1710,7 +1712,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>14</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>14</v>
       </c>
@@ -1744,7 +1746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>14</v>
       </c>
@@ -1761,7 +1763,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>14</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>14</v>
       </c>
@@ -1795,7 +1797,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>14</v>
       </c>
@@ -1812,7 +1814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>15</v>
       </c>
@@ -1829,7 +1831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>15</v>
       </c>
@@ -1846,7 +1848,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>15</v>
       </c>
@@ -1863,7 +1865,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>15</v>
       </c>
@@ -1880,7 +1882,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>15</v>
       </c>
@@ -1897,7 +1899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>15</v>
       </c>
@@ -1914,7 +1916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>15</v>
       </c>
@@ -1931,7 +1933,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>15</v>
       </c>
@@ -1948,7 +1950,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>15</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>15</v>
       </c>
@@ -1982,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>15</v>
       </c>
@@ -1999,7 +2001,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>16</v>
       </c>
@@ -2016,7 +2018,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>16</v>
       </c>
@@ -2033,7 +2035,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>16</v>
       </c>
@@ -2050,7 +2052,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>16</v>
       </c>
@@ -2067,7 +2069,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>16</v>
       </c>
@@ -2084,7 +2086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>16</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>16</v>
       </c>
@@ -2118,7 +2120,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>16</v>
       </c>
@@ -2135,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>18</v>
       </c>
@@ -2152,7 +2154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>20</v>
       </c>
@@ -2169,7 +2171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>20</v>
       </c>
@@ -2186,7 +2188,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>22</v>
       </c>
@@ -2203,7 +2205,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>22</v>
       </c>
@@ -2220,7 +2222,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>22</v>
       </c>
@@ -2237,7 +2239,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>24</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>24</v>
       </c>
@@ -2271,7 +2273,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>25</v>
       </c>
@@ -2288,7 +2290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>25</v>
       </c>
@@ -2305,7 +2307,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>25</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>25</v>
       </c>
@@ -2339,7 +2341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>25</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>25</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>25</v>
       </c>
@@ -2390,7 +2392,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>25</v>
       </c>
@@ -2407,7 +2409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>25</v>
       </c>
@@ -2424,7 +2426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>26</v>
       </c>
@@ -2441,7 +2443,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>27</v>
       </c>
@@ -2458,7 +2460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>27</v>
       </c>
@@ -2475,7 +2477,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5">
       <c r="A117">
         <v>27</v>
       </c>
@@ -2492,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5">
       <c r="A118">
         <v>27</v>
       </c>
@@ -2509,7 +2511,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5">
       <c r="A119">
         <v>28</v>
       </c>
@@ -2526,7 +2528,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5">
       <c r="A120">
         <v>28</v>
       </c>
@@ -2543,7 +2545,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5">
       <c r="A121">
         <v>28</v>
       </c>
@@ -2560,7 +2562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5">
       <c r="A122">
         <v>29</v>
       </c>
@@ -2577,7 +2579,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5">
       <c r="A123">
         <v>30</v>
       </c>
@@ -2594,7 +2596,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5">
       <c r="A124">
         <v>30</v>
       </c>
@@ -2611,7 +2613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5">
       <c r="A125">
         <v>30</v>
       </c>
@@ -2628,7 +2630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5">
       <c r="A126">
         <v>30</v>
       </c>
@@ -2645,7 +2647,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5">
       <c r="A127">
         <v>31</v>
       </c>
@@ -2662,7 +2664,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5">
       <c r="A128">
         <v>31</v>
       </c>
@@ -2679,7 +2681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5">
       <c r="A129">
         <v>31</v>
       </c>
@@ -2696,7 +2698,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5">
       <c r="A130">
         <v>34</v>
       </c>
@@ -2713,7 +2715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5">
       <c r="A131">
         <v>34</v>
       </c>
@@ -2730,7 +2732,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5">
       <c r="A132">
         <v>34</v>
       </c>
@@ -2747,7 +2749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5">
       <c r="A133">
         <v>34</v>
       </c>
@@ -2764,7 +2766,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5">
       <c r="A134">
         <v>34</v>
       </c>
@@ -2781,7 +2783,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5">
       <c r="A135">
         <v>34</v>
       </c>
@@ -2798,7 +2800,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5">
       <c r="A136">
         <v>34</v>
       </c>
@@ -2815,7 +2817,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5">
       <c r="A137">
         <v>35</v>
       </c>
@@ -2832,7 +2834,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5">
       <c r="A138">
         <v>35</v>
       </c>
@@ -2849,7 +2851,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5">
       <c r="A139">
         <v>35</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5">
       <c r="A140">
         <v>35</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5">
       <c r="A141">
         <v>36</v>
       </c>
@@ -2900,7 +2902,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5">
       <c r="A142">
         <v>36</v>
       </c>
@@ -2917,7 +2919,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5">
       <c r="A143">
         <v>36</v>
       </c>
@@ -2934,7 +2936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5">
       <c r="A144">
         <v>36</v>
       </c>
@@ -2951,7 +2953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5">
       <c r="A145">
         <v>36</v>
       </c>
@@ -2968,7 +2970,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5">
       <c r="A146">
         <v>36</v>
       </c>
@@ -2985,7 +2987,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5">
       <c r="A147">
         <v>36</v>
       </c>
@@ -3002,7 +3004,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5">
       <c r="A148">
         <v>36</v>
       </c>
@@ -3019,7 +3021,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5">
       <c r="A149">
         <v>36</v>
       </c>
@@ -3036,7 +3038,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5">
       <c r="A150">
         <v>36</v>
       </c>
@@ -3053,7 +3055,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5">
       <c r="A151">
         <v>36</v>
       </c>
@@ -3070,7 +3072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5">
       <c r="A152">
         <v>36</v>
       </c>
@@ -3087,7 +3089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5">
       <c r="A153">
         <v>38</v>
       </c>
@@ -3104,7 +3106,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5">
       <c r="A154">
         <v>38</v>
       </c>
@@ -3121,7 +3123,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5">
       <c r="A155">
         <v>39</v>
       </c>
@@ -3138,7 +3140,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5">
       <c r="A156">
         <v>40</v>
       </c>
@@ -3155,7 +3157,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5">
       <c r="A157">
         <v>41</v>
       </c>
@@ -3172,7 +3174,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5">
       <c r="A158">
         <v>43</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5">
       <c r="A159">
         <v>43</v>
       </c>
@@ -3206,7 +3208,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5">
       <c r="A160">
         <v>44</v>
       </c>
@@ -3223,7 +3225,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5">
       <c r="A161">
         <v>44</v>
       </c>
@@ -3240,7 +3242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5">
       <c r="A162">
         <v>44</v>
       </c>
@@ -3257,7 +3259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5">
       <c r="A163">
         <v>44</v>
       </c>
@@ -3274,7 +3276,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5">
       <c r="A164">
         <v>44</v>
       </c>
@@ -3291,7 +3293,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5">
       <c r="A165">
         <v>44</v>
       </c>
@@ -3308,7 +3310,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5">
       <c r="A166">
         <v>44</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5">
       <c r="A167">
         <v>44</v>
       </c>
@@ -3342,7 +3344,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5">
       <c r="A168">
         <v>44</v>
       </c>
@@ -3359,7 +3361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5">
       <c r="A169">
         <v>44</v>
       </c>
@@ -3376,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5">
       <c r="A170">
         <v>45</v>
       </c>
@@ -3393,7 +3395,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5">
       <c r="A171">
         <v>45</v>
       </c>
@@ -3410,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5">
       <c r="A172">
         <v>45</v>
       </c>
@@ -3427,7 +3429,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5">
       <c r="A173">
         <v>46</v>
       </c>
@@ -3444,7 +3446,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5">
       <c r="A174">
         <v>46</v>
       </c>
@@ -3461,7 +3463,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5">
       <c r="A175">
         <v>46</v>
       </c>
@@ -3478,7 +3480,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5">
       <c r="A176">
         <v>47</v>
       </c>
@@ -3495,7 +3497,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5">
       <c r="A177">
         <v>50</v>
       </c>
@@ -3512,7 +3514,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5">
       <c r="A178">
         <v>50</v>
       </c>
@@ -3529,7 +3531,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5">
       <c r="A179">
         <v>50</v>
       </c>
@@ -3546,7 +3548,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5">
       <c r="A180">
         <v>51</v>
       </c>
@@ -3563,7 +3565,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5">
       <c r="A181">
         <v>51</v>
       </c>
@@ -3580,7 +3582,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5">
       <c r="A182">
         <v>51</v>
       </c>
@@ -3597,7 +3599,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5">
       <c r="A183">
         <v>51</v>
       </c>
@@ -3614,7 +3616,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5">
       <c r="A184">
         <v>51</v>
       </c>
@@ -3631,7 +3633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5">
       <c r="A185">
         <v>51</v>
       </c>
@@ -3648,7 +3650,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5">
       <c r="A186">
         <v>51</v>
       </c>
@@ -3665,7 +3667,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5">
       <c r="A187">
         <v>51</v>
       </c>
@@ -3682,7 +3684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5">
       <c r="A188">
         <v>51</v>
       </c>
@@ -3699,7 +3701,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5">
       <c r="A189">
         <v>51</v>
       </c>
@@ -3716,7 +3718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5">
       <c r="A190">
         <v>52</v>
       </c>
@@ -3733,7 +3735,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5">
       <c r="A191">
         <v>52</v>
       </c>
@@ -3750,7 +3752,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5">
       <c r="A192">
         <v>52</v>
       </c>
@@ -3767,7 +3769,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5">
       <c r="A193">
         <v>52</v>
       </c>
@@ -3784,7 +3786,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5">
       <c r="A194">
         <v>53</v>
       </c>
@@ -3801,7 +3803,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5">
       <c r="A195">
         <v>53</v>
       </c>
@@ -3818,7 +3820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5">
       <c r="A196">
         <v>53</v>
       </c>
@@ -3835,7 +3837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5">
       <c r="A197">
         <v>53</v>
       </c>
@@ -3852,7 +3854,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5">
       <c r="A198">
         <v>53</v>
       </c>
@@ -3869,7 +3871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5">
       <c r="A199">
         <v>53</v>
       </c>
@@ -3886,7 +3888,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5">
       <c r="A200">
         <v>53</v>
       </c>
@@ -3903,7 +3905,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5">
       <c r="A201">
         <v>53</v>
       </c>
@@ -3920,7 +3922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5">
       <c r="A202">
         <v>53</v>
       </c>
@@ -3937,7 +3939,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5">
       <c r="A203">
         <v>53</v>
       </c>
@@ -3954,7 +3956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5">
       <c r="A204">
         <v>54</v>
       </c>
@@ -3971,7 +3973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5">
       <c r="A205">
         <v>54</v>
       </c>
@@ -3988,7 +3990,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5">
       <c r="A206">
         <v>54</v>
       </c>
@@ -4005,7 +4007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5">
       <c r="A207">
         <v>54</v>
       </c>
@@ -4022,7 +4024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5">
       <c r="A208">
         <v>54</v>
       </c>
@@ -4039,7 +4041,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5">
       <c r="A209">
         <v>54</v>
       </c>
@@ -4056,7 +4058,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5">
       <c r="A210">
         <v>54</v>
       </c>
@@ -4073,7 +4075,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5">
       <c r="A211">
         <v>54</v>
       </c>
@@ -4090,7 +4092,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5">
       <c r="A212">
         <v>54</v>
       </c>
@@ -4107,7 +4109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5">
       <c r="A213">
         <v>55</v>
       </c>
@@ -4124,7 +4126,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5">
       <c r="A214">
         <v>55</v>
       </c>
@@ -4141,7 +4143,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5">
       <c r="A215">
         <v>55</v>
       </c>
@@ -4158,7 +4160,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5">
       <c r="A216">
         <v>56</v>
       </c>
@@ -4175,7 +4177,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5">
       <c r="A217">
         <v>56</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5">
       <c r="A218">
         <v>56</v>
       </c>
@@ -4209,7 +4211,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5">
       <c r="A219">
         <v>56</v>
       </c>
@@ -4226,7 +4228,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5">
       <c r="A220">
         <v>56</v>
       </c>
@@ -4243,7 +4245,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5">
       <c r="A221">
         <v>56</v>
       </c>
@@ -4260,7 +4262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5">
       <c r="A222">
         <v>56</v>
       </c>
@@ -4277,7 +4279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5">
       <c r="A223">
         <v>56</v>
       </c>
@@ -4294,7 +4296,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5">
       <c r="A224">
         <v>56</v>
       </c>
@@ -4311,7 +4313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5">
       <c r="A225">
         <v>56</v>
       </c>
@@ -4328,7 +4330,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5">
       <c r="A226">
         <v>57</v>
       </c>
@@ -4345,7 +4347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5">
       <c r="A227">
         <v>57</v>
       </c>
@@ -4362,7 +4364,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5">
       <c r="A228">
         <v>57</v>
       </c>
@@ -4379,7 +4381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5">
       <c r="A229">
         <v>57</v>
       </c>
@@ -4396,7 +4398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5">
       <c r="A230">
         <v>57</v>
       </c>
@@ -4413,7 +4415,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5">
       <c r="A231">
         <v>57</v>
       </c>
@@ -4430,7 +4432,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5">
       <c r="A232">
         <v>57</v>
       </c>
@@ -4447,7 +4449,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5">
       <c r="A233">
         <v>57</v>
       </c>
@@ -4464,7 +4466,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5">
       <c r="A234">
         <v>57</v>
       </c>
@@ -4481,7 +4483,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5">
       <c r="A235">
         <v>58</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5">
       <c r="A236">
         <v>58</v>
       </c>
@@ -4515,7 +4517,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5">
       <c r="A237">
         <v>59</v>
       </c>
@@ -4532,7 +4534,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5">
       <c r="A238">
         <v>59</v>
       </c>
@@ -4549,7 +4551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5">
       <c r="A239">
         <v>59</v>
       </c>
@@ -4566,7 +4568,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5">
       <c r="A240">
         <v>59</v>
       </c>
@@ -4583,7 +4585,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:6">
       <c r="A241">
         <v>59</v>
       </c>
@@ -4600,7 +4602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:6">
       <c r="A242">
         <v>59</v>
       </c>
@@ -4617,7 +4619,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:6">
       <c r="A243">
         <v>59</v>
       </c>
@@ -4634,7 +4636,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:6">
       <c r="A244">
         <v>60</v>
       </c>
@@ -4651,7 +4653,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:6">
       <c r="A245">
         <v>60</v>
       </c>
@@ -4668,13 +4670,16 @@
         <v>86</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:6">
       <c r="A246">
         <v>61</v>
       </c>
       <c r="B246">
         <v>41</v>
       </c>
+      <c r="C246">
+        <v>61</v>
+      </c>
       <c r="D246">
         <v>7</v>
       </c>
@@ -4685,13 +4690,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:6">
       <c r="A247">
         <v>61</v>
       </c>
       <c r="B247">
         <v>41</v>
       </c>
+      <c r="C247">
+        <v>61</v>
+      </c>
       <c r="D247">
         <v>47</v>
       </c>
@@ -4702,13 +4710,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:6">
       <c r="A248">
         <v>62</v>
       </c>
       <c r="B248">
         <v>18</v>
       </c>
+      <c r="C248">
+        <v>62</v>
+      </c>
       <c r="D248">
         <v>10</v>
       </c>
@@ -4719,13 +4730,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:6">
       <c r="A249">
         <v>62</v>
       </c>
       <c r="B249">
         <v>18</v>
       </c>
+      <c r="C249">
+        <v>62</v>
+      </c>
       <c r="D249">
         <v>20</v>
       </c>
@@ -4736,13 +4750,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:6">
       <c r="A250">
         <v>63</v>
       </c>
       <c r="B250">
         <v>58</v>
       </c>
+      <c r="C250">
+        <v>63</v>
+      </c>
       <c r="D250">
         <v>0</v>
       </c>
@@ -4753,13 +4770,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:6">
       <c r="A251">
         <v>63</v>
       </c>
       <c r="B251">
         <v>58</v>
       </c>
+      <c r="C251">
+        <v>63</v>
+      </c>
       <c r="D251">
         <v>2</v>
       </c>
@@ -4770,13 +4790,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:6">
       <c r="A252">
         <v>63</v>
       </c>
       <c r="B252">
         <v>58</v>
       </c>
+      <c r="C252">
+        <v>63</v>
+      </c>
       <c r="D252">
         <v>4</v>
       </c>
@@ -4787,13 +4810,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:6">
       <c r="A253">
         <v>63</v>
       </c>
       <c r="B253">
         <v>58</v>
       </c>
+      <c r="C253">
+        <v>63</v>
+      </c>
       <c r="D253">
         <v>7</v>
       </c>
@@ -4804,13 +4830,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:6">
       <c r="A254">
         <v>63</v>
       </c>
       <c r="B254">
         <v>58</v>
       </c>
+      <c r="C254">
+        <v>63</v>
+      </c>
       <c r="D254">
         <v>14</v>
       </c>
@@ -4821,13 +4850,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:6">
       <c r="A255">
         <v>63</v>
       </c>
       <c r="B255">
         <v>58</v>
       </c>
+      <c r="C255">
+        <v>63</v>
+      </c>
       <c r="D255">
         <v>16</v>
       </c>
@@ -4838,13 +4870,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:6">
       <c r="A256">
         <v>63</v>
       </c>
       <c r="B256">
         <v>58</v>
       </c>
+      <c r="C256">
+        <v>63</v>
+      </c>
       <c r="D256">
         <v>18</v>
       </c>
@@ -4855,13 +4890,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:6">
       <c r="A257">
         <v>63</v>
       </c>
       <c r="B257">
         <v>58</v>
       </c>
+      <c r="C257">
+        <v>63</v>
+      </c>
       <c r="D257">
         <v>20</v>
       </c>
@@ -4872,13 +4910,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:6">
       <c r="A258">
         <v>63</v>
       </c>
       <c r="B258">
         <v>58</v>
       </c>
+      <c r="C258">
+        <v>63</v>
+      </c>
       <c r="D258">
         <v>25</v>
       </c>
@@ -4889,13 +4930,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:6">
       <c r="A259">
         <v>63</v>
       </c>
       <c r="B259">
         <v>58</v>
       </c>
+      <c r="C259">
+        <v>63</v>
+      </c>
       <c r="D259">
         <v>29</v>
       </c>
@@ -4906,13 +4950,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:6">
       <c r="A260">
         <v>63</v>
       </c>
       <c r="B260">
         <v>58</v>
       </c>
+      <c r="C260">
+        <v>63</v>
+      </c>
       <c r="D260">
         <v>38</v>
       </c>
@@ -4923,13 +4970,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:6">
       <c r="A261">
         <v>63</v>
       </c>
       <c r="B261">
         <v>58</v>
       </c>
+      <c r="C261">
+        <v>63</v>
+      </c>
       <c r="D261">
         <v>39</v>
       </c>
@@ -4940,13 +4990,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:6">
       <c r="A262">
         <v>63</v>
       </c>
       <c r="B262">
         <v>58</v>
       </c>
+      <c r="C262">
+        <v>63</v>
+      </c>
       <c r="D262">
         <v>43</v>
       </c>
@@ -4957,12 +5010,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:6">
       <c r="A263">
         <v>63</v>
       </c>
       <c r="B263">
         <v>58</v>
+      </c>
+      <c r="C263">
+        <v>63</v>
       </c>
       <c r="D263">
         <v>55</v>

</xml_diff>

<commit_message>
revert changes for SampleData
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1975950\Desktop\taor_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBB5DD2-E7AF-4D42-82C1-EBBB291DA7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2153E0B-81F6-4CF3-B40F-64EBC515CF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0DAAF120-E45A-4444-8930-A3E6281725AF}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:F263"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="C246" sqref="C246:C263"/>
+      <selection activeCell="I258" sqref="I258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4677,9 +4677,6 @@
       <c r="B246">
         <v>41</v>
       </c>
-      <c r="C246">
-        <v>61</v>
-      </c>
       <c r="D246">
         <v>7</v>
       </c>
@@ -4697,9 +4694,6 @@
       <c r="B247">
         <v>41</v>
       </c>
-      <c r="C247">
-        <v>61</v>
-      </c>
       <c r="D247">
         <v>47</v>
       </c>
@@ -4717,9 +4711,6 @@
       <c r="B248">
         <v>18</v>
       </c>
-      <c r="C248">
-        <v>62</v>
-      </c>
       <c r="D248">
         <v>10</v>
       </c>
@@ -4737,9 +4728,6 @@
       <c r="B249">
         <v>18</v>
       </c>
-      <c r="C249">
-        <v>62</v>
-      </c>
       <c r="D249">
         <v>20</v>
       </c>
@@ -4757,9 +4745,6 @@
       <c r="B250">
         <v>58</v>
       </c>
-      <c r="C250">
-        <v>63</v>
-      </c>
       <c r="D250">
         <v>0</v>
       </c>
@@ -4777,9 +4762,6 @@
       <c r="B251">
         <v>58</v>
       </c>
-      <c r="C251">
-        <v>63</v>
-      </c>
       <c r="D251">
         <v>2</v>
       </c>
@@ -4797,9 +4779,6 @@
       <c r="B252">
         <v>58</v>
       </c>
-      <c r="C252">
-        <v>63</v>
-      </c>
       <c r="D252">
         <v>4</v>
       </c>
@@ -4817,9 +4796,6 @@
       <c r="B253">
         <v>58</v>
       </c>
-      <c r="C253">
-        <v>63</v>
-      </c>
       <c r="D253">
         <v>7</v>
       </c>
@@ -4837,9 +4813,6 @@
       <c r="B254">
         <v>58</v>
       </c>
-      <c r="C254">
-        <v>63</v>
-      </c>
       <c r="D254">
         <v>14</v>
       </c>
@@ -4857,9 +4830,6 @@
       <c r="B255">
         <v>58</v>
       </c>
-      <c r="C255">
-        <v>63</v>
-      </c>
       <c r="D255">
         <v>16</v>
       </c>
@@ -4877,9 +4847,6 @@
       <c r="B256">
         <v>58</v>
       </c>
-      <c r="C256">
-        <v>63</v>
-      </c>
       <c r="D256">
         <v>18</v>
       </c>
@@ -4897,9 +4864,6 @@
       <c r="B257">
         <v>58</v>
       </c>
-      <c r="C257">
-        <v>63</v>
-      </c>
       <c r="D257">
         <v>20</v>
       </c>
@@ -4917,9 +4881,6 @@
       <c r="B258">
         <v>58</v>
       </c>
-      <c r="C258">
-        <v>63</v>
-      </c>
       <c r="D258">
         <v>25</v>
       </c>
@@ -4937,9 +4898,6 @@
       <c r="B259">
         <v>58</v>
       </c>
-      <c r="C259">
-        <v>63</v>
-      </c>
       <c r="D259">
         <v>29</v>
       </c>
@@ -4957,9 +4915,6 @@
       <c r="B260">
         <v>58</v>
       </c>
-      <c r="C260">
-        <v>63</v>
-      </c>
       <c r="D260">
         <v>38</v>
       </c>
@@ -4977,9 +4932,6 @@
       <c r="B261">
         <v>58</v>
       </c>
-      <c r="C261">
-        <v>63</v>
-      </c>
       <c r="D261">
         <v>39</v>
       </c>
@@ -4997,9 +4949,6 @@
       <c r="B262">
         <v>58</v>
       </c>
-      <c r="C262">
-        <v>63</v>
-      </c>
       <c r="D262">
         <v>43</v>
       </c>
@@ -5016,9 +4965,6 @@
       </c>
       <c r="B263">
         <v>58</v>
-      </c>
-      <c r="C263">
-        <v>63</v>
       </c>
       <c r="D263">
         <v>55</v>

</xml_diff>